<commit_message>
Add meaningful markers for LArTPC and Cherenkov Ring
</commit_message>
<xml_diff>
--- a/tools/MakeJsons/ExpList.xlsx
+++ b/tools/MakeJsons/ExpList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maco/Documents/Apps/Webpages/NeutrinoExperimentsOnEarth/MakeJsons/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maco/Documents/Apps/Webpages/NeutrinoExperimentsOnEarth/tools/MakeJsons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194C8B93-5BD3-A84D-B94D-E255A5973DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBFA643-1091-F04D-BF26-57E735881675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="740" windowWidth="28320" windowHeight="18380" xr2:uid="{07D09D20-4562-D946-BD27-9B78457AD267}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="113">
   <si>
     <t>Name</t>
   </si>
@@ -372,6 +372,9 @@
   </si>
   <si>
     <t>Micro-Booster Neutrino Experiment</t>
+  </si>
+  <si>
+    <t>https://johncarlosbaez.wordpress.com/wp-content/uploads/2018/06/a-schematic-drawing-of-the-miniboone-detector.png</t>
   </si>
 </sst>
 </file>
@@ -824,7 +827,7 @@
   <dimension ref="A1:AI1096"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1321,7 +1324,9 @@
       <c r="E9" s="1">
         <v>-88.269498139999996</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="G9" s="2" t="s">
         <v>55</v>
       </c>

</xml_diff>